<commit_message>
Corrected error in ceiling jet spreasheet; one test was taking incorrect columns for relative difference
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/Analysis/CompareListPyroGraph.xlsx
+++ b/cfast/trunk/Validation/Analysis/CompareListPyroGraph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="9240" windowHeight="9945" tabRatio="743" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9240" windowHeight="9945" tabRatio="743" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Processed Output" sheetId="17" r:id="rId1"/>
@@ -1724,16 +1724,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1757,15 +1793,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1777,12 +1804,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1804,27 +1825,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1840,6 +1840,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1847,14 +1849,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1872,6 +1866,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -17646,17 +17646,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" s="4" customFormat="1">
-      <c r="C2" s="197" t="s">
+      <c r="C2" s="177" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1" ht="25.5">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="178" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="33" t="s">
@@ -17670,8 +17670,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="13" customFormat="1" ht="14.25">
-      <c r="A4" s="172"/>
-      <c r="B4" s="172"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="181"/>
       <c r="C4" s="39" t="s">
         <v>50</v>
       </c>
@@ -17683,7 +17683,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="200" t="s">
+      <c r="A5" s="172" t="s">
         <v>157</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -17703,7 +17703,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="201"/>
+      <c r="A6" s="173"/>
       <c r="B6" s="8" t="s">
         <v>29</v>
       </c>
@@ -17721,7 +17721,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="201"/>
+      <c r="A7" s="173"/>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
@@ -17739,7 +17739,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="201"/>
+      <c r="A8" s="173"/>
       <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
@@ -17757,7 +17757,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="201"/>
+      <c r="A9" s="173"/>
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
@@ -17775,7 +17775,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="201"/>
+      <c r="A10" s="173"/>
       <c r="B10" s="8" t="s">
         <v>32</v>
       </c>
@@ -17793,7 +17793,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="201"/>
+      <c r="A11" s="173"/>
       <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
@@ -17811,7 +17811,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="201"/>
+      <c r="A12" s="173"/>
       <c r="B12" s="8" t="s">
         <v>36</v>
       </c>
@@ -17829,7 +17829,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="201"/>
+      <c r="A13" s="173"/>
       <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
@@ -17847,7 +17847,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="201"/>
+      <c r="A14" s="173"/>
       <c r="B14" s="8" t="s">
         <v>26</v>
       </c>
@@ -17865,7 +17865,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="201"/>
+      <c r="A15" s="173"/>
       <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
@@ -17883,7 +17883,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="201"/>
+      <c r="A16" s="173"/>
       <c r="B16" s="8" t="s">
         <v>28</v>
       </c>
@@ -17901,7 +17901,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="201"/>
+      <c r="A17" s="173"/>
       <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
@@ -17919,7 +17919,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="201"/>
+      <c r="A18" s="173"/>
       <c r="B18" s="8" t="s">
         <v>35</v>
       </c>
@@ -17937,7 +17937,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="201"/>
+      <c r="A19" s="173"/>
       <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
@@ -18088,7 +18088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -18102,18 +18102,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" s="4" customFormat="1">
-      <c r="C2" s="197" t="s">
+      <c r="C2" s="177" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
       <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" s="12" customFormat="1" ht="25.5">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="178" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="33" t="s">
@@ -18128,8 +18128,8 @@
       <c r="G3" s="89"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1">
-      <c r="A4" s="172"/>
-      <c r="B4" s="172"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="181"/>
       <c r="C4" s="38" t="s">
         <v>51</v>
       </c>
@@ -18142,7 +18142,7 @@
       <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="200" t="s">
+      <c r="A5" s="172" t="s">
         <v>157</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -18166,7 +18166,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="201"/>
+      <c r="A6" s="173"/>
       <c r="B6" s="8" t="s">
         <v>29</v>
       </c>
@@ -18188,7 +18188,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="201"/>
+      <c r="A7" s="173"/>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
@@ -18210,7 +18210,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="201"/>
+      <c r="A8" s="173"/>
       <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
@@ -18232,7 +18232,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="201"/>
+      <c r="A9" s="173"/>
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
@@ -18254,7 +18254,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="201"/>
+      <c r="A10" s="173"/>
       <c r="B10" s="8" t="s">
         <v>32</v>
       </c>
@@ -18276,7 +18276,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="201"/>
+      <c r="A11" s="173"/>
       <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
@@ -18298,7 +18298,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="201"/>
+      <c r="A12" s="173"/>
       <c r="B12" s="8" t="s">
         <v>36</v>
       </c>
@@ -18320,7 +18320,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="201"/>
+      <c r="A13" s="173"/>
       <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
@@ -18342,7 +18342,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="201"/>
+      <c r="A14" s="173"/>
       <c r="B14" s="8" t="s">
         <v>26</v>
       </c>
@@ -18364,7 +18364,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="201"/>
+      <c r="A15" s="173"/>
       <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
@@ -18386,7 +18386,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="201"/>
+      <c r="A16" s="173"/>
       <c r="B16" s="8" t="s">
         <v>28</v>
       </c>
@@ -18408,7 +18408,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="201"/>
+      <c r="A17" s="173"/>
       <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
@@ -18430,7 +18430,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="201"/>
+      <c r="A18" s="173"/>
       <c r="B18" s="8" t="s">
         <v>35</v>
       </c>
@@ -18452,7 +18452,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="201"/>
+      <c r="A19" s="173"/>
       <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
@@ -18498,7 +18498,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="199"/>
+      <c r="A21" s="180"/>
       <c r="B21" s="54" t="s">
         <v>128</v>
       </c>
@@ -18659,21 +18659,21 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1">
-      <c r="D2" s="197" t="s">
+      <c r="D2" s="177" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197" t="s">
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
-      <c r="J2" s="197" t="s">
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="197"/>
-      <c r="L2" s="197"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
       <c r="N2" s="84" t="s">
         <v>142</v>
       </c>
@@ -18685,11 +18685,11 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="12" customFormat="1">
-      <c r="A3" s="171"/>
-      <c r="B3" s="202" t="s">
+      <c r="A3" s="178"/>
+      <c r="B3" s="182" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="171" t="s">
+      <c r="C3" s="178" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="29" t="s">
@@ -18727,9 +18727,9 @@
       <c r="P3" s="89"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="14.25">
-      <c r="A4" s="172"/>
-      <c r="B4" s="172"/>
-      <c r="C4" s="172"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
       <c r="D4" s="42" t="s">
         <v>52</v>
       </c>
@@ -18765,7 +18765,7 @@
       <c r="P4" s="37"/>
     </row>
     <row r="5" spans="1:16" customFormat="1">
-      <c r="A5" s="196" t="s">
+      <c r="A5" s="203" t="s">
         <v>157</v>
       </c>
       <c r="B5" s="223" t="s">
@@ -18824,7 +18824,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" customFormat="1">
-      <c r="A6" s="193"/>
+      <c r="A6" s="200"/>
       <c r="B6" s="207"/>
       <c r="C6" s="128" t="s">
         <v>308</v>
@@ -18879,7 +18879,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" customFormat="1">
-      <c r="A7" s="193"/>
+      <c r="A7" s="200"/>
       <c r="B7" s="207"/>
       <c r="C7" s="128" t="s">
         <v>311</v>
@@ -18934,7 +18934,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" customFormat="1">
-      <c r="A8" s="193"/>
+      <c r="A8" s="200"/>
       <c r="B8" s="207"/>
       <c r="C8" s="128" t="s">
         <v>310</v>
@@ -18989,7 +18989,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" customFormat="1">
-      <c r="A9" s="193"/>
+      <c r="A9" s="200"/>
       <c r="B9" s="207"/>
       <c r="C9" s="128" t="s">
         <v>313</v>
@@ -19044,7 +19044,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" customFormat="1">
-      <c r="A10" s="193"/>
+      <c r="A10" s="200"/>
       <c r="B10" s="207"/>
       <c r="C10" s="128" t="s">
         <v>307</v>
@@ -19099,7 +19099,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" customFormat="1">
-      <c r="A11" s="193"/>
+      <c r="A11" s="200"/>
       <c r="B11" s="207"/>
       <c r="C11" s="128" t="s">
         <v>309</v>
@@ -19154,7 +19154,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" customFormat="1">
-      <c r="A12" s="193"/>
+      <c r="A12" s="200"/>
       <c r="B12" s="207"/>
       <c r="C12" s="128" t="s">
         <v>312</v>
@@ -19209,7 +19209,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" customFormat="1">
-      <c r="A13" s="193"/>
+      <c r="A13" s="200"/>
       <c r="B13" s="207"/>
       <c r="C13" s="127" t="s">
         <v>32</v>
@@ -19264,7 +19264,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" customFormat="1">
-      <c r="A14" s="193"/>
+      <c r="A14" s="200"/>
       <c r="B14" s="207"/>
       <c r="C14" s="127" t="s">
         <v>33</v>
@@ -19292,7 +19292,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" customFormat="1">
-      <c r="A15" s="193"/>
+      <c r="A15" s="200"/>
       <c r="B15" s="207"/>
       <c r="C15" s="127" t="s">
         <v>34</v>
@@ -19347,7 +19347,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" customFormat="1">
-      <c r="A16" s="193"/>
+      <c r="A16" s="200"/>
       <c r="B16" s="207"/>
       <c r="C16" s="127" t="s">
         <v>35</v>
@@ -19402,7 +19402,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" customFormat="1">
-      <c r="A17" s="193"/>
+      <c r="A17" s="200"/>
       <c r="B17" s="207"/>
       <c r="C17" s="127" t="s">
         <v>36</v>
@@ -19457,7 +19457,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" customFormat="1">
-      <c r="A18" s="193"/>
+      <c r="A18" s="200"/>
       <c r="B18" s="207"/>
       <c r="C18" s="127" t="s">
         <v>37</v>
@@ -19485,7 +19485,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" customFormat="1">
-      <c r="A19" s="193"/>
+      <c r="A19" s="200"/>
       <c r="B19" s="208"/>
       <c r="C19" s="127" t="s">
         <v>38</v>
@@ -19540,7 +19540,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" customFormat="1">
-      <c r="A20" s="193"/>
+      <c r="A20" s="200"/>
       <c r="B20" s="223" t="s">
         <v>315</v>
       </c>
@@ -19570,7 +19570,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" customFormat="1">
-      <c r="A21" s="193"/>
+      <c r="A21" s="200"/>
       <c r="B21" s="207"/>
       <c r="C21" s="128" t="s">
         <v>308</v>
@@ -19625,7 +19625,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" customFormat="1">
-      <c r="A22" s="193"/>
+      <c r="A22" s="200"/>
       <c r="B22" s="207"/>
       <c r="C22" s="128" t="s">
         <v>311</v>
@@ -19662,7 +19662,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" customFormat="1">
-      <c r="A23" s="193"/>
+      <c r="A23" s="200"/>
       <c r="B23" s="207"/>
       <c r="C23" s="128" t="s">
         <v>310</v>
@@ -19717,7 +19717,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" customFormat="1">
-      <c r="A24" s="193"/>
+      <c r="A24" s="200"/>
       <c r="B24" s="207"/>
       <c r="C24" s="128" t="s">
         <v>313</v>
@@ -19772,7 +19772,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" customFormat="1">
-      <c r="A25" s="193"/>
+      <c r="A25" s="200"/>
       <c r="B25" s="207"/>
       <c r="C25" s="128" t="s">
         <v>307</v>
@@ -19827,7 +19827,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" customFormat="1">
-      <c r="A26" s="193"/>
+      <c r="A26" s="200"/>
       <c r="B26" s="207"/>
       <c r="C26" s="128" t="s">
         <v>309</v>
@@ -19882,7 +19882,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" customFormat="1">
-      <c r="A27" s="193"/>
+      <c r="A27" s="200"/>
       <c r="B27" s="207"/>
       <c r="C27" s="128" t="s">
         <v>312</v>
@@ -19937,7 +19937,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" customFormat="1">
-      <c r="A28" s="193"/>
+      <c r="A28" s="200"/>
       <c r="B28" s="207"/>
       <c r="C28" s="127" t="s">
         <v>32</v>
@@ -19992,7 +19992,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" customFormat="1">
-      <c r="A29" s="193"/>
+      <c r="A29" s="200"/>
       <c r="B29" s="207"/>
       <c r="C29" s="127" t="s">
         <v>33</v>
@@ -20047,7 +20047,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" customFormat="1">
-      <c r="A30" s="193"/>
+      <c r="A30" s="200"/>
       <c r="B30" s="207"/>
       <c r="C30" s="127" t="s">
         <v>34</v>
@@ -20102,7 +20102,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" customFormat="1">
-      <c r="A31" s="193"/>
+      <c r="A31" s="200"/>
       <c r="B31" s="207"/>
       <c r="C31" s="127" t="s">
         <v>35</v>
@@ -20139,7 +20139,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" customFormat="1">
-      <c r="A32" s="193"/>
+      <c r="A32" s="200"/>
       <c r="B32" s="207"/>
       <c r="C32" s="127" t="s">
         <v>36</v>
@@ -20194,7 +20194,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" customFormat="1">
-      <c r="A33" s="193"/>
+      <c r="A33" s="200"/>
       <c r="B33" s="207"/>
       <c r="C33" s="127" t="s">
         <v>37</v>
@@ -20222,7 +20222,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" customFormat="1">
-      <c r="A34" s="193"/>
+      <c r="A34" s="200"/>
       <c r="B34" s="208"/>
       <c r="C34" s="127" t="s">
         <v>38</v>
@@ -20259,7 +20259,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" customFormat="1">
-      <c r="A35" s="193"/>
+      <c r="A35" s="200"/>
       <c r="B35" s="223" t="s">
         <v>316</v>
       </c>
@@ -20316,7 +20316,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" customFormat="1">
-      <c r="A36" s="193"/>
+      <c r="A36" s="200"/>
       <c r="B36" s="207"/>
       <c r="C36" s="128" t="s">
         <v>308</v>
@@ -20371,7 +20371,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" customFormat="1">
-      <c r="A37" s="193"/>
+      <c r="A37" s="200"/>
       <c r="B37" s="207"/>
       <c r="C37" s="128" t="s">
         <v>311</v>
@@ -20426,7 +20426,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" customFormat="1">
-      <c r="A38" s="193"/>
+      <c r="A38" s="200"/>
       <c r="B38" s="207"/>
       <c r="C38" s="128" t="s">
         <v>310</v>
@@ -20481,7 +20481,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" customFormat="1">
-      <c r="A39" s="193"/>
+      <c r="A39" s="200"/>
       <c r="B39" s="207"/>
       <c r="C39" s="128" t="s">
         <v>313</v>
@@ -20536,7 +20536,7 @@
       </c>
     </row>
     <row r="40" spans="1:16" customFormat="1">
-      <c r="A40" s="193"/>
+      <c r="A40" s="200"/>
       <c r="B40" s="207"/>
       <c r="C40" s="128" t="s">
         <v>307</v>
@@ -20591,7 +20591,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" customFormat="1">
-      <c r="A41" s="193"/>
+      <c r="A41" s="200"/>
       <c r="B41" s="207"/>
       <c r="C41" s="128" t="s">
         <v>309</v>
@@ -20646,7 +20646,7 @@
       </c>
     </row>
     <row r="42" spans="1:16" customFormat="1">
-      <c r="A42" s="193"/>
+      <c r="A42" s="200"/>
       <c r="B42" s="207"/>
       <c r="C42" s="128" t="s">
         <v>312</v>
@@ -20701,7 +20701,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" customFormat="1">
-      <c r="A43" s="193"/>
+      <c r="A43" s="200"/>
       <c r="B43" s="207"/>
       <c r="C43" s="127" t="s">
         <v>32</v>
@@ -20756,7 +20756,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" customFormat="1">
-      <c r="A44" s="193"/>
+      <c r="A44" s="200"/>
       <c r="B44" s="207"/>
       <c r="C44" s="127" t="s">
         <v>33</v>
@@ -20811,7 +20811,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" customFormat="1">
-      <c r="A45" s="193"/>
+      <c r="A45" s="200"/>
       <c r="B45" s="207"/>
       <c r="C45" s="127" t="s">
         <v>34</v>
@@ -20866,7 +20866,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" customFormat="1">
-      <c r="A46" s="193"/>
+      <c r="A46" s="200"/>
       <c r="B46" s="207"/>
       <c r="C46" s="127" t="s">
         <v>35</v>
@@ -20921,7 +20921,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" customFormat="1">
-      <c r="A47" s="193"/>
+      <c r="A47" s="200"/>
       <c r="B47" s="207"/>
       <c r="C47" s="127" t="s">
         <v>36</v>
@@ -20976,7 +20976,7 @@
       </c>
     </row>
     <row r="48" spans="1:16" customFormat="1">
-      <c r="A48" s="193"/>
+      <c r="A48" s="200"/>
       <c r="B48" s="207"/>
       <c r="C48" s="127" t="s">
         <v>37</v>
@@ -21004,7 +21004,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" customFormat="1">
-      <c r="A49" s="193"/>
+      <c r="A49" s="200"/>
       <c r="B49" s="208"/>
       <c r="C49" s="127" t="s">
         <v>38</v>
@@ -21059,7 +21059,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" customFormat="1">
-      <c r="A50" s="193"/>
+      <c r="A50" s="200"/>
       <c r="B50" s="223" t="s">
         <v>317</v>
       </c>
@@ -21107,7 +21107,7 @@
       </c>
     </row>
     <row r="51" spans="1:16" customFormat="1">
-      <c r="A51" s="193"/>
+      <c r="A51" s="200"/>
       <c r="B51" s="207"/>
       <c r="C51" s="128" t="s">
         <v>308</v>
@@ -21153,7 +21153,7 @@
       </c>
     </row>
     <row r="52" spans="1:16" customFormat="1">
-      <c r="A52" s="193"/>
+      <c r="A52" s="200"/>
       <c r="B52" s="207"/>
       <c r="C52" s="128" t="s">
         <v>311</v>
@@ -21208,7 +21208,7 @@
       </c>
     </row>
     <row r="53" spans="1:16" customFormat="1">
-      <c r="A53" s="193"/>
+      <c r="A53" s="200"/>
       <c r="B53" s="207"/>
       <c r="C53" s="128" t="s">
         <v>310</v>
@@ -21263,7 +21263,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" customFormat="1">
-      <c r="A54" s="193"/>
+      <c r="A54" s="200"/>
       <c r="B54" s="207"/>
       <c r="C54" s="128" t="s">
         <v>313</v>
@@ -21318,7 +21318,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" customFormat="1">
-      <c r="A55" s="193"/>
+      <c r="A55" s="200"/>
       <c r="B55" s="207"/>
       <c r="C55" s="128" t="s">
         <v>307</v>
@@ -21373,7 +21373,7 @@
       </c>
     </row>
     <row r="56" spans="1:16" customFormat="1">
-      <c r="A56" s="193"/>
+      <c r="A56" s="200"/>
       <c r="B56" s="207"/>
       <c r="C56" s="128" t="s">
         <v>309</v>
@@ -21428,7 +21428,7 @@
       </c>
     </row>
     <row r="57" spans="1:16" customFormat="1">
-      <c r="A57" s="193"/>
+      <c r="A57" s="200"/>
       <c r="B57" s="207"/>
       <c r="C57" s="128" t="s">
         <v>312</v>
@@ -21483,7 +21483,7 @@
       </c>
     </row>
     <row r="58" spans="1:16" customFormat="1">
-      <c r="A58" s="193"/>
+      <c r="A58" s="200"/>
       <c r="B58" s="207"/>
       <c r="C58" s="127" t="s">
         <v>32</v>
@@ -21538,7 +21538,7 @@
       </c>
     </row>
     <row r="59" spans="1:16" customFormat="1">
-      <c r="A59" s="193"/>
+      <c r="A59" s="200"/>
       <c r="B59" s="207"/>
       <c r="C59" s="127" t="s">
         <v>33</v>
@@ -21593,7 +21593,7 @@
       </c>
     </row>
     <row r="60" spans="1:16" customFormat="1">
-      <c r="A60" s="193"/>
+      <c r="A60" s="200"/>
       <c r="B60" s="207"/>
       <c r="C60" s="127" t="s">
         <v>34</v>
@@ -21648,7 +21648,7 @@
       </c>
     </row>
     <row r="61" spans="1:16" customFormat="1">
-      <c r="A61" s="193"/>
+      <c r="A61" s="200"/>
       <c r="B61" s="207"/>
       <c r="C61" s="127" t="s">
         <v>35</v>
@@ -22026,17 +22026,17 @@
     <sortCondition ref="B5:B64"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="A5:A64"/>
-    <mergeCell ref="B5:B19"/>
-    <mergeCell ref="B20:B34"/>
-    <mergeCell ref="B35:B49"/>
-    <mergeCell ref="B50:B64"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="A5:A64"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="B20:B34"/>
+    <mergeCell ref="B35:B49"/>
+    <mergeCell ref="B50:B64"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -22095,13 +22095,13 @@
       <c r="C3" s="226" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197" t="s">
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="197"/>
-      <c r="H3" s="197"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
       <c r="J3" s="136" t="s">
         <v>149</v>
       </c>
@@ -22110,10 +22110,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="12" customFormat="1" ht="25.5">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="182" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="178" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="29" t="s">
@@ -22142,8 +22142,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="14.25">
-      <c r="A5" s="172"/>
-      <c r="B5" s="172"/>
+      <c r="A5" s="181"/>
+      <c r="B5" s="181"/>
       <c r="C5" s="39" t="s">
         <v>52</v>
       </c>
@@ -24458,14 +24458,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="A51:A65"/>
+    <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A20"/>
     <mergeCell ref="A21:A35"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="A51:A65"/>
-    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24478,7 +24478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J594"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A160" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -49446,7 +49446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -49549,11 +49549,11 @@
       </c>
       <c r="D7" s="143">
         <f>'Plume Temp'!H27*100</f>
-        <v>20.8</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E7" s="143">
         <f>'Plume Temp'!H28</f>
-        <v>41.187183999999995</v>
+        <v>41.183942999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -49562,19 +49562,19 @@
       </c>
       <c r="B8" s="143">
         <f>'Ceiling Jet'!F28</f>
-        <v>32.852231578947368</v>
+        <v>14.506738947368424</v>
       </c>
       <c r="C8" s="143">
         <f>'Ceiling Jet'!H30</f>
-        <v>7.9423300000000001</v>
+        <v>3.9573299999999998</v>
       </c>
       <c r="D8" s="143">
         <f>'Ceiling Jet'!H31*100</f>
-        <v>78.3</v>
+        <v>83.899999999999991</v>
       </c>
       <c r="E8" s="143">
         <f>'Ceiling Jet'!H32</f>
-        <v>100.36643599999998</v>
+        <v>34.921197999999947</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -50906,11 +50906,11 @@
       </c>
       <c r="F15" s="59">
         <f>IF('Ceiling Jet'!D12&lt;&gt;"",'Ceiling Jet'!D12,"")</f>
-        <v>370.435</v>
+        <v>344</v>
       </c>
       <c r="G15" s="59">
         <f>IF('Ceiling Jet'!E12&lt;&gt;"",'Ceiling Jet'!E12,"")</f>
-        <v>344</v>
+        <v>350.435</v>
       </c>
       <c r="J15" s="59">
         <f>IF('Gas Concentration'!G11&lt;&gt;"",'Gas Concentration'!G11,"")</f>
@@ -58258,7 +58258,7 @@
       </c>
       <c r="N12" s="59">
         <f>IF('Ceiling Jet'!F12&lt;&gt;"",'Ceiling Jet'!F12,"")</f>
-        <v>350.435</v>
+        <v>1.8706400000000001</v>
       </c>
       <c r="R12" s="59">
         <f>IF('Gas Concentration'!I11&lt;&gt;"",'Gas Concentration'!I11,"")</f>
@@ -60462,7 +60462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
@@ -60482,26 +60482,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="K1" s="189" t="s">
+      <c r="K1" s="196" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="189"/>
-      <c r="O1" s="169" t="s">
+      <c r="L1" s="196"/>
+      <c r="O1" s="183" t="s">
         <v>133</v>
       </c>
-      <c r="P1" s="170"/>
+      <c r="P1" s="184"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="25.5">
-      <c r="D2" s="197" t="s">
+      <c r="D2" s="177" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197" t="s">
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
       <c r="K2" s="92" t="s">
         <v>1</v>
       </c>
@@ -60517,13 +60517,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="12" customFormat="1" ht="25.5">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="171" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="202" t="s">
+      <c r="B3" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="182" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
@@ -60552,7 +60552,7 @@
         <f>I3</f>
         <v>Relative Difference</v>
       </c>
-      <c r="N3" s="171" t="s">
+      <c r="N3" s="178" t="s">
         <v>17</v>
       </c>
       <c r="O3" s="31" t="str">
@@ -60565,9 +60565,9 @@
       </c>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1">
-      <c r="A4" s="172"/>
-      <c r="B4" s="172"/>
-      <c r="C4" s="172"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
       <c r="D4" s="30" t="s">
         <v>22</v>
       </c>
@@ -60594,7 +60594,7 @@
         <f>I4</f>
         <v>(%)</v>
       </c>
-      <c r="N4" s="172"/>
+      <c r="N4" s="181"/>
       <c r="O4" s="31" t="str">
         <f>I4</f>
         <v>(%)</v>
@@ -60605,7 +60605,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="12.75" customHeight="1">
-      <c r="A5" s="171" t="s">
+      <c r="A5" s="178" t="s">
         <v>156</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -60635,7 +60635,7 @@
         <f>IF(I5&lt;&gt;"",ABS(I5),"")</f>
         <v/>
       </c>
-      <c r="N5" s="192" t="s">
+      <c r="N5" s="199" t="s">
         <v>18</v>
       </c>
       <c r="O5" s="24">
@@ -60648,7 +60648,7 @@
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="198"/>
+      <c r="A6" s="179"/>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
@@ -60676,12 +60676,12 @@
         <f t="shared" ref="L6:L60" si="1">IF(I6&lt;&gt;"",ABS(I6),"")</f>
         <v/>
       </c>
-      <c r="N6" s="193"/>
+      <c r="N6" s="200"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="199"/>
+      <c r="A7" s="180"/>
       <c r="B7" s="8" t="s">
         <v>21</v>
       </c>
@@ -60718,12 +60718,12 @@
         <f t="shared" si="1"/>
         <v>7.4961799999999998</v>
       </c>
-      <c r="N7" s="194"/>
+      <c r="N7" s="201"/>
       <c r="O7" s="86"/>
       <c r="P7" s="86"/>
     </row>
     <row r="8" spans="1:16" ht="12.75" customHeight="1">
-      <c r="A8" s="200" t="s">
+      <c r="A8" s="172" t="s">
         <v>157</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -60753,7 +60753,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N8" s="192" t="s">
+      <c r="N8" s="199" t="s">
         <v>39</v>
       </c>
       <c r="O8" s="24">
@@ -60766,7 +60766,7 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="201"/>
+      <c r="A9" s="173"/>
       <c r="B9" s="8" t="s">
         <v>29</v>
       </c>
@@ -60794,12 +60794,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N9" s="193"/>
+      <c r="N9" s="200"/>
       <c r="O9" s="85"/>
       <c r="P9" s="85"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="201"/>
+      <c r="A10" s="173"/>
       <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
@@ -60827,12 +60827,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N10" s="193"/>
+      <c r="N10" s="200"/>
       <c r="O10" s="85"/>
       <c r="P10" s="85"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="201"/>
+      <c r="A11" s="173"/>
       <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
@@ -60860,12 +60860,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N11" s="193"/>
+      <c r="N11" s="200"/>
       <c r="O11" s="85"/>
       <c r="P11" s="85"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="201"/>
+      <c r="A12" s="173"/>
       <c r="B12" s="8" t="s">
         <v>27</v>
       </c>
@@ -60893,12 +60893,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N12" s="193"/>
+      <c r="N12" s="200"/>
       <c r="O12" s="85"/>
       <c r="P12" s="85"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="201"/>
+      <c r="A13" s="173"/>
       <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
@@ -60926,12 +60926,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N13" s="193"/>
+      <c r="N13" s="200"/>
       <c r="O13" s="85"/>
       <c r="P13" s="85"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="201"/>
+      <c r="A14" s="173"/>
       <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
@@ -60959,12 +60959,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N14" s="193"/>
+      <c r="N14" s="200"/>
       <c r="O14" s="85"/>
       <c r="P14" s="85"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="201"/>
+      <c r="A15" s="173"/>
       <c r="B15" s="8" t="s">
         <v>36</v>
       </c>
@@ -60992,12 +60992,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N15" s="193"/>
+      <c r="N15" s="200"/>
       <c r="O15" s="85"/>
       <c r="P15" s="85"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="201"/>
+      <c r="A16" s="173"/>
       <c r="B16" s="8" t="s">
         <v>37</v>
       </c>
@@ -61025,12 +61025,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N16" s="193"/>
+      <c r="N16" s="200"/>
       <c r="O16" s="85"/>
       <c r="P16" s="85"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="201"/>
+      <c r="A17" s="173"/>
       <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
@@ -61067,12 +61067,12 @@
         <f t="shared" si="1"/>
         <v>4.9821400000000002</v>
       </c>
-      <c r="N17" s="193"/>
+      <c r="N17" s="200"/>
       <c r="O17" s="85"/>
       <c r="P17" s="85"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="201"/>
+      <c r="A18" s="173"/>
       <c r="B18" s="8" t="s">
         <v>31</v>
       </c>
@@ -61109,12 +61109,12 @@
         <f t="shared" si="1"/>
         <v>5.8195199999999998</v>
       </c>
-      <c r="N18" s="193"/>
+      <c r="N18" s="200"/>
       <c r="O18" s="85"/>
       <c r="P18" s="85"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="201"/>
+      <c r="A19" s="173"/>
       <c r="B19" s="8" t="s">
         <v>28</v>
       </c>
@@ -61151,12 +61151,12 @@
         <f t="shared" si="1"/>
         <v>14.196070000000001</v>
       </c>
-      <c r="N19" s="193"/>
+      <c r="N19" s="200"/>
       <c r="O19" s="85"/>
       <c r="P19" s="85"/>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="201"/>
+      <c r="A20" s="173"/>
       <c r="B20" s="8" t="s">
         <v>34</v>
       </c>
@@ -61193,12 +61193,12 @@
         <f t="shared" si="1"/>
         <v>5.3553300000000004</v>
       </c>
-      <c r="N20" s="193"/>
+      <c r="N20" s="200"/>
       <c r="O20" s="85"/>
       <c r="P20" s="85"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="201"/>
+      <c r="A21" s="173"/>
       <c r="B21" s="8" t="s">
         <v>35</v>
       </c>
@@ -61235,12 +61235,12 @@
         <f t="shared" si="1"/>
         <v>5.2408400000000004</v>
       </c>
-      <c r="N21" s="193"/>
+      <c r="N21" s="200"/>
       <c r="O21" s="85"/>
       <c r="P21" s="85"/>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="201"/>
+      <c r="A22" s="173"/>
       <c r="B22" s="8" t="s">
         <v>38</v>
       </c>
@@ -61277,7 +61277,7 @@
         <f t="shared" si="1"/>
         <v>5.1773199999999999</v>
       </c>
-      <c r="N22" s="194"/>
+      <c r="N22" s="201"/>
       <c r="O22" s="86"/>
       <c r="P22" s="86"/>
     </row>
@@ -61386,7 +61386,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="12.75" customHeight="1">
-      <c r="A25" s="179" t="s">
+      <c r="A25" s="191" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -61416,7 +61416,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N25" s="183" t="s">
+      <c r="N25" s="192" t="s">
         <v>42</v>
       </c>
       <c r="O25" s="24">
@@ -61426,7 +61426,7 @@
       <c r="P25" s="24"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="179"/>
+      <c r="A26" s="191"/>
       <c r="B26" s="8" t="s">
         <v>28</v>
       </c>
@@ -61454,12 +61454,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N26" s="184"/>
+      <c r="N26" s="193"/>
       <c r="O26" s="85"/>
       <c r="P26" s="85"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="179"/>
+      <c r="A27" s="191"/>
       <c r="B27" s="8" t="s">
         <v>44</v>
       </c>
@@ -61487,15 +61487,15 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N27" s="195"/>
+      <c r="N27" s="202"/>
       <c r="O27" s="86"/>
       <c r="P27" s="86"/>
     </row>
     <row r="28" spans="1:16" ht="12.75" customHeight="1">
-      <c r="A28" s="200" t="s">
+      <c r="A28" s="172" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="187" t="s">
+      <c r="B28" s="171" t="s">
         <v>122</v>
       </c>
       <c r="C28" s="53" t="s">
@@ -61533,7 +61533,7 @@
         <f t="shared" si="1"/>
         <v>30.869050000000001</v>
       </c>
-      <c r="N28" s="196" t="s">
+      <c r="N28" s="203" t="s">
         <v>123</v>
       </c>
       <c r="O28" s="17">
@@ -61546,8 +61546,8 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="201"/>
-      <c r="B29" s="188"/>
+      <c r="A29" s="173"/>
+      <c r="B29" s="170"/>
       <c r="C29" s="53" t="s">
         <v>117</v>
       </c>
@@ -61583,13 +61583,13 @@
         <f t="shared" si="1"/>
         <v>16.422440000000002</v>
       </c>
-      <c r="N29" s="190"/>
+      <c r="N29" s="197"/>
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="201"/>
-      <c r="B30" s="188"/>
+      <c r="A30" s="173"/>
+      <c r="B30" s="170"/>
       <c r="C30" s="53" t="s">
         <v>117</v>
       </c>
@@ -61625,13 +61625,13 @@
         <f t="shared" si="1"/>
         <v>16.363959999999999</v>
       </c>
-      <c r="N30" s="190"/>
+      <c r="N30" s="197"/>
       <c r="O30" s="85"/>
       <c r="P30" s="85"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="201"/>
-      <c r="B31" s="188"/>
+      <c r="A31" s="173"/>
+      <c r="B31" s="170"/>
       <c r="C31" s="53" t="s">
         <v>117</v>
       </c>
@@ -61667,13 +61667,13 @@
         <f t="shared" si="1"/>
         <v>19.97963</v>
       </c>
-      <c r="N31" s="190"/>
+      <c r="N31" s="197"/>
       <c r="O31" s="85"/>
       <c r="P31" s="85"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="201"/>
-      <c r="B32" s="188"/>
+      <c r="A32" s="173"/>
+      <c r="B32" s="170"/>
       <c r="C32" s="55" t="s">
         <v>121</v>
       </c>
@@ -61709,13 +61709,13 @@
         <f t="shared" si="1"/>
         <v>21.057259999999999</v>
       </c>
-      <c r="N32" s="190"/>
+      <c r="N32" s="197"/>
       <c r="O32" s="85"/>
       <c r="P32" s="85"/>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="201"/>
-      <c r="B33" s="188"/>
+      <c r="A33" s="173"/>
+      <c r="B33" s="170"/>
       <c r="C33" s="53" t="s">
         <v>120</v>
       </c>
@@ -61751,13 +61751,13 @@
         <f t="shared" si="1"/>
         <v>16.370080000000002</v>
       </c>
-      <c r="N33" s="190"/>
+      <c r="N33" s="197"/>
       <c r="O33" s="85"/>
       <c r="P33" s="85"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="201"/>
-      <c r="B34" s="187" t="s">
+      <c r="A34" s="173"/>
+      <c r="B34" s="171" t="s">
         <v>124</v>
       </c>
       <c r="C34" s="53" t="s">
@@ -61795,13 +61795,13 @@
         <f t="shared" si="1"/>
         <v>3.9900500000000001</v>
       </c>
-      <c r="N34" s="190"/>
+      <c r="N34" s="197"/>
       <c r="O34" s="85"/>
       <c r="P34" s="85"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="201"/>
-      <c r="B35" s="188"/>
+      <c r="A35" s="173"/>
+      <c r="B35" s="170"/>
       <c r="C35" s="53" t="s">
         <v>117</v>
       </c>
@@ -61837,13 +61837,13 @@
         <f t="shared" si="1"/>
         <v>13.09066</v>
       </c>
-      <c r="N35" s="190"/>
+      <c r="N35" s="197"/>
       <c r="O35" s="85"/>
       <c r="P35" s="85"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="201"/>
-      <c r="B36" s="188"/>
+      <c r="A36" s="173"/>
+      <c r="B36" s="170"/>
       <c r="C36" s="53" t="s">
         <v>117</v>
       </c>
@@ -61879,13 +61879,13 @@
         <f t="shared" si="1"/>
         <v>13.09066</v>
       </c>
-      <c r="N36" s="190"/>
+      <c r="N36" s="197"/>
       <c r="O36" s="85"/>
       <c r="P36" s="85"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="201"/>
-      <c r="B37" s="188"/>
+      <c r="A37" s="173"/>
+      <c r="B37" s="170"/>
       <c r="C37" s="53" t="s">
         <v>117</v>
       </c>
@@ -61921,13 +61921,13 @@
         <f t="shared" si="1"/>
         <v>16.40063</v>
       </c>
-      <c r="N37" s="190"/>
+      <c r="N37" s="197"/>
       <c r="O37" s="85"/>
       <c r="P37" s="85"/>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="201"/>
-      <c r="B38" s="188"/>
+      <c r="A38" s="173"/>
+      <c r="B38" s="170"/>
       <c r="C38" s="55" t="s">
         <v>121</v>
       </c>
@@ -61963,13 +61963,13 @@
         <f t="shared" si="1"/>
         <v>14.54166</v>
       </c>
-      <c r="N38" s="190"/>
+      <c r="N38" s="197"/>
       <c r="O38" s="85"/>
       <c r="P38" s="85"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="201"/>
-      <c r="B39" s="188"/>
+      <c r="A39" s="173"/>
+      <c r="B39" s="170"/>
       <c r="C39" s="53" t="s">
         <v>120</v>
       </c>
@@ -62005,15 +62005,15 @@
         <f t="shared" si="1"/>
         <v>13.73198</v>
       </c>
-      <c r="N39" s="191"/>
+      <c r="N39" s="198"/>
       <c r="O39" s="86"/>
       <c r="P39" s="86"/>
     </row>
     <row r="40" spans="1:16" ht="12.75" customHeight="1">
-      <c r="A40" s="183" t="s">
+      <c r="A40" s="192" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="180" t="s">
+      <c r="B40" s="174" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="9" t="s">
@@ -62051,7 +62051,7 @@
         <f t="shared" si="1"/>
         <v>7.9115900000000003</v>
       </c>
-      <c r="N40" s="183" t="s">
+      <c r="N40" s="192" t="s">
         <v>43</v>
       </c>
       <c r="O40" s="24">
@@ -62064,8 +62064,8 @@
       </c>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="184"/>
-      <c r="B41" s="181"/>
+      <c r="A41" s="193"/>
+      <c r="B41" s="175"/>
       <c r="C41" s="9" t="s">
         <v>62</v>
       </c>
@@ -62101,13 +62101,13 @@
         <f t="shared" si="1"/>
         <v>5.7706799999999996</v>
       </c>
-      <c r="N41" s="190"/>
+      <c r="N41" s="197"/>
       <c r="O41" s="85"/>
       <c r="P41" s="85"/>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="184"/>
-      <c r="B42" s="181"/>
+      <c r="A42" s="193"/>
+      <c r="B42" s="175"/>
       <c r="C42" s="9" t="s">
         <v>63</v>
       </c>
@@ -62143,13 +62143,13 @@
         <f t="shared" si="1"/>
         <v>8.5219000000000005</v>
       </c>
-      <c r="N42" s="190"/>
+      <c r="N42" s="197"/>
       <c r="O42" s="85"/>
       <c r="P42" s="85"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="184"/>
-      <c r="B43" s="182"/>
+      <c r="A43" s="193"/>
+      <c r="B43" s="176"/>
       <c r="C43" s="9" t="s">
         <v>46</v>
       </c>
@@ -62185,13 +62185,13 @@
         <f t="shared" si="1"/>
         <v>15.32095</v>
       </c>
-      <c r="N43" s="190"/>
+      <c r="N43" s="197"/>
       <c r="O43" s="85"/>
       <c r="P43" s="85"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="184"/>
-      <c r="B44" s="180" t="s">
+      <c r="A44" s="193"/>
+      <c r="B44" s="174" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="9" t="s">
@@ -62220,13 +62220,13 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N44" s="190"/>
+      <c r="N44" s="197"/>
       <c r="O44" s="85"/>
       <c r="P44" s="85"/>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="184"/>
-      <c r="B45" s="181"/>
+      <c r="A45" s="193"/>
+      <c r="B45" s="175"/>
       <c r="C45" s="9" t="s">
         <v>62</v>
       </c>
@@ -62253,13 +62253,13 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N45" s="190"/>
+      <c r="N45" s="197"/>
       <c r="O45" s="85"/>
       <c r="P45" s="85"/>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="184"/>
-      <c r="B46" s="181"/>
+      <c r="A46" s="193"/>
+      <c r="B46" s="175"/>
       <c r="C46" s="9" t="s">
         <v>63</v>
       </c>
@@ -62286,13 +62286,13 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N46" s="190"/>
+      <c r="N46" s="197"/>
       <c r="O46" s="85"/>
       <c r="P46" s="85"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="184"/>
-      <c r="B47" s="182"/>
+      <c r="A47" s="193"/>
+      <c r="B47" s="176"/>
       <c r="C47" s="9" t="s">
         <v>46</v>
       </c>
@@ -62319,13 +62319,13 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N47" s="190"/>
+      <c r="N47" s="197"/>
       <c r="O47" s="85"/>
       <c r="P47" s="85"/>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="184"/>
-      <c r="B48" s="180" t="s">
+      <c r="A48" s="193"/>
+      <c r="B48" s="174" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -62363,13 +62363,13 @@
         <f t="shared" si="1"/>
         <v>14.38406</v>
       </c>
-      <c r="N48" s="190"/>
+      <c r="N48" s="197"/>
       <c r="O48" s="85"/>
       <c r="P48" s="85"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="184"/>
-      <c r="B49" s="181"/>
+      <c r="A49" s="193"/>
+      <c r="B49" s="175"/>
       <c r="C49" s="9" t="s">
         <v>62</v>
       </c>
@@ -62405,13 +62405,13 @@
         <f t="shared" si="1"/>
         <v>15.757490000000001</v>
       </c>
-      <c r="N49" s="190"/>
+      <c r="N49" s="197"/>
       <c r="O49" s="85"/>
       <c r="P49" s="85"/>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="184"/>
-      <c r="B50" s="181"/>
+      <c r="A50" s="193"/>
+      <c r="B50" s="175"/>
       <c r="C50" s="9" t="s">
         <v>63</v>
       </c>
@@ -62447,13 +62447,13 @@
         <f t="shared" si="1"/>
         <v>27.430499999999999</v>
       </c>
-      <c r="N50" s="190"/>
+      <c r="N50" s="197"/>
       <c r="O50" s="85"/>
       <c r="P50" s="85"/>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="184"/>
-      <c r="B51" s="182"/>
+      <c r="A51" s="193"/>
+      <c r="B51" s="176"/>
       <c r="C51" s="9" t="s">
         <v>47</v>
       </c>
@@ -62489,16 +62489,16 @@
         <f t="shared" si="1"/>
         <v>73.554079999999999</v>
       </c>
-      <c r="N51" s="190"/>
+      <c r="N51" s="197"/>
       <c r="O51" s="86"/>
       <c r="P51" s="86"/>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="185"/>
-      <c r="B52" s="187" t="s">
+      <c r="A52" s="194"/>
+      <c r="B52" s="171" t="s">
         <v>125</v>
       </c>
-      <c r="C52" s="203" t="s">
+      <c r="C52" s="169" t="s">
         <v>45</v>
       </c>
       <c r="D52" s="10">
@@ -62533,7 +62533,7 @@
         <f t="shared" si="1"/>
         <v>0.70892999999999995</v>
       </c>
-      <c r="N52" s="190"/>
+      <c r="N52" s="197"/>
       <c r="O52" s="24">
         <f>AVERAGE(K52:K55)</f>
         <v>17.262854999999998</v>
@@ -62544,9 +62544,9 @@
       </c>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="185"/>
-      <c r="B53" s="188"/>
-      <c r="C53" s="188"/>
+      <c r="A53" s="194"/>
+      <c r="B53" s="170"/>
+      <c r="C53" s="170"/>
       <c r="D53" s="10">
         <f>'Sorted Output'!H374</f>
         <v>897.25</v>
@@ -62579,16 +62579,16 @@
         <f t="shared" si="1"/>
         <v>7.7068300000000001</v>
       </c>
-      <c r="N53" s="190"/>
+      <c r="N53" s="197"/>
       <c r="O53" s="85"/>
       <c r="P53" s="85"/>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="185"/>
-      <c r="B54" s="187" t="s">
+      <c r="A54" s="194"/>
+      <c r="B54" s="171" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="203" t="s">
+      <c r="C54" s="169" t="s">
         <v>45</v>
       </c>
       <c r="D54" s="10">
@@ -62623,14 +62623,14 @@
         <f t="shared" si="1"/>
         <v>7.9138500000000001</v>
       </c>
-      <c r="N54" s="190"/>
+      <c r="N54" s="197"/>
       <c r="O54" s="85"/>
       <c r="P54" s="85"/>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="185"/>
-      <c r="B55" s="188"/>
-      <c r="C55" s="188"/>
+      <c r="A55" s="194"/>
+      <c r="B55" s="170"/>
+      <c r="C55" s="170"/>
       <c r="D55" s="10">
         <f>'Sorted Output'!H376</f>
         <v>878.32</v>
@@ -62663,12 +62663,12 @@
         <f t="shared" si="1"/>
         <v>42.811669999999999</v>
       </c>
-      <c r="N55" s="190"/>
+      <c r="N55" s="197"/>
       <c r="O55" s="86"/>
       <c r="P55" s="86"/>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="185"/>
+      <c r="A56" s="194"/>
       <c r="B56" s="54" t="s">
         <v>127</v>
       </c>
@@ -62707,7 +62707,7 @@
         <f t="shared" si="1"/>
         <v>104.90864999999999</v>
       </c>
-      <c r="N56" s="190"/>
+      <c r="N56" s="197"/>
       <c r="O56" s="24">
         <f>AVERAGE(K56:K57)</f>
         <v>38.226424999999999</v>
@@ -62718,7 +62718,7 @@
       </c>
     </row>
     <row r="57" spans="1:16">
-      <c r="A57" s="186"/>
+      <c r="A57" s="195"/>
       <c r="B57" s="54" t="s">
         <v>128</v>
       </c>
@@ -62757,15 +62757,15 @@
         <f t="shared" si="1"/>
         <v>106.62669</v>
       </c>
-      <c r="N57" s="191"/>
+      <c r="N57" s="198"/>
       <c r="O57" s="86"/>
       <c r="P57" s="86"/>
     </row>
     <row r="58" spans="1:16" ht="12.75" customHeight="1">
-      <c r="A58" s="173" t="s">
+      <c r="A58" s="185" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="176" t="s">
+      <c r="B58" s="188" t="s">
         <v>29</v>
       </c>
       <c r="C58" s="53" t="s">
@@ -62794,7 +62794,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N58" s="173" t="s">
+      <c r="N58" s="185" t="s">
         <v>119</v>
       </c>
       <c r="O58" s="24">
@@ -62804,8 +62804,8 @@
       <c r="P58" s="24"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="174"/>
-      <c r="B59" s="177"/>
+      <c r="A59" s="186"/>
+      <c r="B59" s="189"/>
       <c r="C59" s="53" t="s">
         <v>117</v>
       </c>
@@ -62832,13 +62832,13 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N59" s="190"/>
+      <c r="N59" s="197"/>
       <c r="O59" s="85"/>
       <c r="P59" s="85"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="175"/>
-      <c r="B60" s="178"/>
+      <c r="A60" s="187"/>
+      <c r="B60" s="190"/>
       <c r="C60" s="53" t="s">
         <v>118</v>
       </c>
@@ -62865,7 +62865,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N60" s="191"/>
+      <c r="N60" s="198"/>
       <c r="O60" s="86"/>
       <c r="P60" s="86"/>
     </row>
@@ -63002,20 +63002,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="A28:A39"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A22"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="C3:C4"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="A58:A60"/>
@@ -63032,6 +63018,20 @@
     <mergeCell ref="N25:N27"/>
     <mergeCell ref="N28:N39"/>
     <mergeCell ref="N40:N57"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A22"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="A28:A39"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B48:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -63049,7 +63049,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H12" sqref="H12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -63073,11 +63073,11 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" ht="25.5">
-      <c r="D2" s="197" t="s">
+      <c r="D2" s="177" t="s">
         <v>159</v>
       </c>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
       <c r="H2" s="92" t="s">
         <v>160</v>
       </c>
@@ -63087,13 +63087,13 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="12" customFormat="1" ht="25.5">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="171" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="202" t="s">
+      <c r="B3" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="182" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="29" t="s">
@@ -63109,7 +63109,7 @@
         <f>F3</f>
         <v>Relative Difference</v>
       </c>
-      <c r="J3" s="171" t="s">
+      <c r="J3" s="178" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="31" t="str">
@@ -63118,9 +63118,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1">
-      <c r="A4" s="172"/>
-      <c r="B4" s="172"/>
-      <c r="C4" s="172"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
       <c r="D4" s="30" t="s">
         <v>22</v>
       </c>
@@ -63134,17 +63134,17 @@
         <f>F4</f>
         <v>(%)</v>
       </c>
-      <c r="J4" s="172"/>
+      <c r="J4" s="181"/>
       <c r="K4" s="37" t="str">
         <f>H4</f>
         <v>(%)</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A5" s="171" t="s">
+      <c r="A5" s="178" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="180" t="s">
+      <c r="B5" s="174" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="123" t="s">
@@ -63166,7 +63166,7 @@
         <f>IF(F5&lt;&gt;"",ABS(F5),"")</f>
         <v>41.206629999999997</v>
       </c>
-      <c r="J5" s="171" t="s">
+      <c r="J5" s="178" t="s">
         <v>156</v>
       </c>
       <c r="K5" s="204">
@@ -63175,8 +63175,8 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="198"/>
-      <c r="B6" s="182"/>
+      <c r="A6" s="179"/>
+      <c r="B6" s="176"/>
       <c r="C6" s="123" t="s">
         <v>162</v>
       </c>
@@ -63196,12 +63196,12 @@
         <f t="shared" ref="H6:H22" si="0">IF(F6&lt;&gt;"",ABS(F6),"")</f>
         <v>40.792400000000001</v>
       </c>
-      <c r="J6" s="198"/>
+      <c r="J6" s="179"/>
       <c r="K6" s="205"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="198"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="179"/>
+      <c r="B7" s="174" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="123" t="s">
@@ -63223,12 +63223,12 @@
         <f t="shared" si="0"/>
         <v>30.487159999999999</v>
       </c>
-      <c r="J7" s="198"/>
+      <c r="J7" s="179"/>
       <c r="K7" s="205"/>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A8" s="181"/>
-      <c r="B8" s="182"/>
+      <c r="A8" s="175"/>
+      <c r="B8" s="176"/>
       <c r="C8" s="123" t="s">
         <v>162</v>
       </c>
@@ -63248,12 +63248,12 @@
         <f t="shared" si="0"/>
         <v>41.174219999999998</v>
       </c>
-      <c r="J8" s="181"/>
+      <c r="J8" s="175"/>
       <c r="K8" s="205"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="181"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="175"/>
+      <c r="B9" s="174" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="123" t="s">
@@ -63275,12 +63275,12 @@
         <f t="shared" si="0"/>
         <v>29.00198</v>
       </c>
-      <c r="J9" s="181"/>
+      <c r="J9" s="175"/>
       <c r="K9" s="205"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="182"/>
-      <c r="B10" s="182"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="176"/>
       <c r="C10" s="123" t="s">
         <v>162</v>
       </c>
@@ -63300,11 +63300,11 @@
         <f t="shared" si="0"/>
         <v>26.563559999999999</v>
       </c>
-      <c r="J10" s="182"/>
+      <c r="J10" s="176"/>
       <c r="K10" s="206"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="179" t="s">
+      <c r="A11" s="191" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -63329,16 +63329,16 @@
         <f t="shared" si="0"/>
         <v>7.2202200000000003</v>
       </c>
-      <c r="J11" s="179" t="s">
+      <c r="J11" s="191" t="s">
         <v>42</v>
       </c>
       <c r="K11" s="204">
         <f>AVERAGE(H11:H13)</f>
-        <v>13.377170000000001</v>
+        <v>15.264083333333334</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="179"/>
+      <c r="A12" s="191"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
@@ -63361,11 +63361,11 @@
         <f t="shared" si="0"/>
         <v>19.534120000000001</v>
       </c>
-      <c r="J12" s="179"/>
+      <c r="J12" s="191"/>
       <c r="K12" s="205"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="179"/>
+      <c r="A13" s="191"/>
       <c r="B13" s="8" t="s">
         <v>44</v>
       </c>
@@ -63384,12 +63384,15 @@
         <f>'Sorted Output'!J499</f>
         <v>19.03791</v>
       </c>
-      <c r="H13" s="94"/>
-      <c r="J13" s="179"/>
+      <c r="H13" s="94">
+        <f t="shared" si="0"/>
+        <v>19.03791</v>
+      </c>
+      <c r="J13" s="191"/>
       <c r="K13" s="206"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="185" t="s">
         <v>208</v>
       </c>
       <c r="B14" s="123" t="s">
@@ -63414,7 +63417,7 @@
         <f t="shared" si="0"/>
         <v>73.182680000000005</v>
       </c>
-      <c r="J14" s="183" t="str">
+      <c r="J14" s="192" t="str">
         <f>A14</f>
         <v>NIST High Bay</v>
       </c>
@@ -63447,7 +63450,7 @@
         <f t="shared" si="0"/>
         <v>36.751559999999998</v>
       </c>
-      <c r="J15" s="184"/>
+      <c r="J15" s="193"/>
       <c r="K15" s="205"/>
     </row>
     <row r="16" spans="1:11">
@@ -63474,7 +63477,7 @@
         <f t="shared" si="0"/>
         <v>5.4253400000000003</v>
       </c>
-      <c r="J16" s="184"/>
+      <c r="J16" s="193"/>
       <c r="K16" s="205"/>
     </row>
     <row r="17" spans="1:11">
@@ -63501,7 +63504,7 @@
         <f t="shared" si="0"/>
         <v>19.03791</v>
       </c>
-      <c r="J17" s="184"/>
+      <c r="J17" s="193"/>
       <c r="K17" s="205"/>
     </row>
     <row r="18" spans="1:11">
@@ -63528,7 +63531,7 @@
         <f t="shared" si="0"/>
         <v>19.81738</v>
       </c>
-      <c r="J18" s="184"/>
+      <c r="J18" s="193"/>
       <c r="K18" s="205"/>
     </row>
     <row r="19" spans="1:11">
@@ -63555,7 +63558,7 @@
         <f t="shared" si="0"/>
         <v>15.832409999999999</v>
       </c>
-      <c r="J19" s="184"/>
+      <c r="J19" s="193"/>
       <c r="K19" s="205"/>
     </row>
     <row r="20" spans="1:11">
@@ -63582,7 +63585,7 @@
         <f t="shared" si="0"/>
         <v>24.273109999999999</v>
       </c>
-      <c r="J20" s="184"/>
+      <c r="J20" s="193"/>
       <c r="K20" s="205"/>
     </row>
     <row r="21" spans="1:11">
@@ -63609,7 +63612,7 @@
         <f t="shared" si="0"/>
         <v>13.04311</v>
       </c>
-      <c r="J21" s="184"/>
+      <c r="J21" s="193"/>
       <c r="K21" s="205"/>
     </row>
     <row r="22" spans="1:11">
@@ -63636,7 +63639,7 @@
         <f t="shared" si="0"/>
         <v>8.4418199999999999</v>
       </c>
-      <c r="J22" s="195"/>
+      <c r="J22" s="202"/>
       <c r="K22" s="206"/>
     </row>
     <row r="23" spans="1:11">
@@ -63709,7 +63712,7 @@
       <c r="G27" s="97"/>
       <c r="H27" s="100">
         <f>PERCENTRANK(H5:H22,14)</f>
-        <v>0.20799999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -63724,16 +63727,11 @@
       <c r="G28" s="97"/>
       <c r="H28" s="101">
         <f>PERCENTILE(H5:H22,0.9)</f>
-        <v>41.187183999999995</v>
+        <v>41.183942999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="J3:J4"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K5:K10"/>
     <mergeCell ref="A14:A22"/>
@@ -63746,6 +63744,11 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="J5:J10"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -63758,8 +63761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25:H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -63781,11 +63784,11 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="197" t="s">
+      <c r="D3" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
       <c r="H3" s="82" t="s">
         <v>131</v>
       </c>
@@ -63793,18 +63796,18 @@
       <c r="J3" s="88"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="209"/>
-      <c r="N3" s="210"/>
-      <c r="O3" s="211"/>
+      <c r="M3" s="211"/>
+      <c r="N3" s="212"/>
+      <c r="O3" s="213"/>
     </row>
     <row r="4" spans="1:16" ht="25.5">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="171" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="202" t="s">
+      <c r="B4" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="182" t="s">
         <v>48</v>
       </c>
       <c r="D4" s="29" t="s">
@@ -63819,13 +63822,13 @@
       <c r="H4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="171" t="s">
+      <c r="J4" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="171" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="202" t="s">
+      <c r="K4" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="182" t="s">
         <v>48</v>
       </c>
       <c r="M4" s="29" t="s">
@@ -63839,9 +63842,9 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="172"/>
-      <c r="B5" s="172"/>
-      <c r="C5" s="172"/>
+      <c r="A5" s="181"/>
+      <c r="B5" s="181"/>
+      <c r="C5" s="181"/>
       <c r="D5" s="30" t="s">
         <v>22</v>
       </c>
@@ -63854,9 +63857,9 @@
       <c r="H5" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="172"/>
-      <c r="K5" s="172"/>
-      <c r="L5" s="172"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="181"/>
       <c r="M5" s="30" t="s">
         <v>22</v>
       </c>
@@ -63868,7 +63871,7 @@
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="200" t="s">
+      <c r="A6" s="172" t="s">
         <v>157</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -63892,7 +63895,7 @@
         <v>11.33419</v>
       </c>
       <c r="I6" s="47"/>
-      <c r="J6" s="201" t="s">
+      <c r="J6" s="173" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="8" t="s">
@@ -63914,7 +63917,7 @@
       <c r="P6" s="47"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="201"/>
+      <c r="A7" s="173"/>
       <c r="B7" s="8" t="s">
         <v>29</v>
       </c>
@@ -63935,7 +63938,7 @@
         <f t="shared" ref="H7:H24" si="0">ABS(F7)</f>
         <v>3.5418500000000002</v>
       </c>
-      <c r="J7" s="201"/>
+      <c r="J7" s="173"/>
       <c r="K7" s="8" t="s">
         <v>29</v>
       </c>
@@ -63954,7 +63957,7 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="201"/>
+      <c r="A8" s="173"/>
       <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
@@ -63975,7 +63978,7 @@
         <f t="shared" si="0"/>
         <v>7.9423300000000001</v>
       </c>
-      <c r="J8" s="201"/>
+      <c r="J8" s="173"/>
       <c r="K8" s="8" t="s">
         <v>25</v>
       </c>
@@ -63994,7 +63997,7 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="201"/>
+      <c r="A9" s="173"/>
       <c r="B9" s="8" t="s">
         <v>30</v>
       </c>
@@ -64015,7 +64018,7 @@
         <f t="shared" si="0"/>
         <v>3.2600799999999999</v>
       </c>
-      <c r="J9" s="201"/>
+      <c r="J9" s="173"/>
       <c r="K9" s="8" t="s">
         <v>30</v>
       </c>
@@ -64034,7 +64037,7 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="201"/>
+      <c r="A10" s="173"/>
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
@@ -64055,7 +64058,7 @@
         <f t="shared" si="0"/>
         <v>3.9573299999999998</v>
       </c>
-      <c r="J10" s="201"/>
+      <c r="J10" s="173"/>
       <c r="K10" s="8" t="s">
         <v>27</v>
       </c>
@@ -64074,7 +64077,7 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="201"/>
+      <c r="A11" s="173"/>
       <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
@@ -64095,7 +64098,7 @@
         <f t="shared" si="0"/>
         <v>9.2463499999999996</v>
       </c>
-      <c r="J11" s="201"/>
+      <c r="J11" s="173"/>
       <c r="K11" s="8" t="s">
         <v>32</v>
       </c>
@@ -64114,35 +64117,35 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="201"/>
+      <c r="A12" s="173"/>
       <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="16">
-        <f>'Sorted Output'!G192</f>
-        <v>370.435</v>
-      </c>
-      <c r="E12" s="16">
         <f>'Sorted Output'!H192</f>
         <v>344</v>
       </c>
-      <c r="F12" s="121">
+      <c r="E12" s="16">
         <f>'Sorted Output'!I192</f>
         <v>350.435</v>
       </c>
+      <c r="F12" s="16">
+        <f>'Sorted Output'!J192</f>
+        <v>1.8706400000000001</v>
+      </c>
       <c r="H12" s="32">
         <f t="shared" si="0"/>
-        <v>350.435</v>
-      </c>
-      <c r="J12" s="201"/>
+        <v>1.8706400000000001</v>
+      </c>
+      <c r="J12" s="173"/>
       <c r="K12" s="8" t="s">
         <v>33</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="16">
         <f t="shared" si="1"/>
-        <v>370.435</v>
+        <v>344</v>
       </c>
       <c r="N12" s="16">
         <f>'HGT &amp; HGL'!D14</f>
@@ -64150,11 +64153,11 @@
       </c>
       <c r="O12" s="17">
         <f t="shared" si="2"/>
-        <v>79.975000000000023</v>
+        <v>53.54000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="201"/>
+      <c r="A13" s="173"/>
       <c r="B13" s="8" t="s">
         <v>36</v>
       </c>
@@ -64175,7 +64178,7 @@
         <f t="shared" si="0"/>
         <v>15.533810000000001</v>
       </c>
-      <c r="J13" s="201"/>
+      <c r="J13" s="173"/>
       <c r="K13" s="8" t="s">
         <v>36</v>
       </c>
@@ -64194,7 +64197,7 @@
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="201"/>
+      <c r="A14" s="173"/>
       <c r="B14" s="8" t="s">
         <v>37</v>
       </c>
@@ -64215,7 +64218,7 @@
         <f t="shared" si="0"/>
         <v>1.17625</v>
       </c>
-      <c r="J14" s="201"/>
+      <c r="J14" s="173"/>
       <c r="K14" s="8" t="s">
         <v>37</v>
       </c>
@@ -64234,7 +64237,7 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="201"/>
+      <c r="A15" s="173"/>
       <c r="B15" s="8" t="s">
         <v>26</v>
       </c>
@@ -64255,7 +64258,7 @@
         <f t="shared" si="0"/>
         <v>3.21129</v>
       </c>
-      <c r="J15" s="201"/>
+      <c r="J15" s="173"/>
       <c r="K15" s="8" t="s">
         <v>26</v>
       </c>
@@ -64274,7 +64277,7 @@
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="201"/>
+      <c r="A16" s="173"/>
       <c r="B16" s="8" t="s">
         <v>31</v>
       </c>
@@ -64295,7 +64298,7 @@
         <f t="shared" si="0"/>
         <v>3.2512300000000001</v>
       </c>
-      <c r="J16" s="201"/>
+      <c r="J16" s="173"/>
       <c r="K16" s="8" t="s">
         <v>31</v>
       </c>
@@ -64314,7 +64317,7 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="201"/>
+      <c r="A17" s="173"/>
       <c r="B17" s="8" t="s">
         <v>28</v>
       </c>
@@ -64335,7 +64338,7 @@
         <f t="shared" si="0"/>
         <v>1.19194</v>
       </c>
-      <c r="J17" s="201"/>
+      <c r="J17" s="173"/>
       <c r="K17" s="8" t="s">
         <v>28</v>
       </c>
@@ -64354,7 +64357,7 @@
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="201"/>
+      <c r="A18" s="173"/>
       <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
@@ -64375,7 +64378,7 @@
         <f t="shared" si="0"/>
         <v>0.88785000000000003</v>
       </c>
-      <c r="J18" s="201"/>
+      <c r="J18" s="173"/>
       <c r="K18" s="8" t="s">
         <v>34</v>
       </c>
@@ -64394,7 +64397,7 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="201"/>
+      <c r="A19" s="173"/>
       <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
@@ -64415,7 +64418,7 @@
         <f t="shared" si="0"/>
         <v>2.8963399999999999</v>
       </c>
-      <c r="J19" s="201"/>
+      <c r="J19" s="173"/>
       <c r="K19" s="8" t="s">
         <v>35</v>
       </c>
@@ -64434,7 +64437,7 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="201"/>
+      <c r="A20" s="173"/>
       <c r="B20" s="8" t="s">
         <v>38</v>
       </c>
@@ -64455,7 +64458,7 @@
         <f t="shared" si="0"/>
         <v>11.800840000000001</v>
       </c>
-      <c r="J20" s="201"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="8" t="s">
         <v>38</v>
       </c>
@@ -64474,10 +64477,10 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="183" t="s">
+      <c r="A21" s="192" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="180" t="s">
+      <c r="B21" s="174" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -64499,10 +64502,10 @@
         <f t="shared" si="0"/>
         <v>13.93901</v>
       </c>
-      <c r="J21" s="183" t="s">
+      <c r="J21" s="192" t="s">
         <v>42</v>
       </c>
-      <c r="K21" s="180" t="s">
+      <c r="K21" s="174" t="s">
         <v>27</v>
       </c>
       <c r="L21" s="8" t="s">
@@ -64523,8 +64526,8 @@
       <c r="P21" s="47"/>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="184"/>
-      <c r="B22" s="182"/>
+      <c r="A22" s="193"/>
+      <c r="B22" s="176"/>
       <c r="C22" s="8" t="s">
         <v>112</v>
       </c>
@@ -64544,8 +64547,8 @@
         <f t="shared" si="0"/>
         <v>94.445350000000005</v>
       </c>
-      <c r="J22" s="184"/>
-      <c r="K22" s="182"/>
+      <c r="J22" s="193"/>
+      <c r="K22" s="176"/>
       <c r="L22" s="8" t="s">
         <v>112</v>
       </c>
@@ -64563,8 +64566,8 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="184"/>
-      <c r="B23" s="180" t="s">
+      <c r="A23" s="193"/>
+      <c r="B23" s="174" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -64586,8 +64589,8 @@
         <f t="shared" si="0"/>
         <v>20.04016</v>
       </c>
-      <c r="J23" s="184"/>
-      <c r="K23" s="180" t="s">
+      <c r="J23" s="193"/>
+      <c r="K23" s="174" t="s">
         <v>28</v>
       </c>
       <c r="L23" s="8" t="s">
@@ -64607,8 +64610,8 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="212"/>
-      <c r="B24" s="182"/>
+      <c r="A24" s="209"/>
+      <c r="B24" s="176"/>
       <c r="C24" s="8" t="s">
         <v>112</v>
       </c>
@@ -64628,8 +64631,8 @@
         <f t="shared" si="0"/>
         <v>124.05078</v>
       </c>
-      <c r="J24" s="212"/>
-      <c r="K24" s="182"/>
+      <c r="J24" s="209"/>
+      <c r="K24" s="176"/>
       <c r="L24" s="8" t="s">
         <v>112</v>
       </c>
@@ -64647,8 +64650,8 @@
       </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="212"/>
-      <c r="B25" s="180" t="s">
+      <c r="A25" s="209"/>
+      <c r="B25" s="174" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -64658,8 +64661,8 @@
       <c r="E25" s="16"/>
       <c r="F25" s="121"/>
       <c r="H25" s="32"/>
-      <c r="J25" s="212"/>
-      <c r="K25" s="180" t="s">
+      <c r="J25" s="209"/>
+      <c r="K25" s="174" t="s">
         <v>44</v>
       </c>
       <c r="L25" s="8" t="s">
@@ -64679,8 +64682,8 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="213"/>
-      <c r="B26" s="182"/>
+      <c r="A26" s="210"/>
+      <c r="B26" s="176"/>
       <c r="C26" s="8" t="s">
         <v>112</v>
       </c>
@@ -64688,8 +64691,8 @@
       <c r="E26" s="16"/>
       <c r="F26" s="121"/>
       <c r="H26" s="32"/>
-      <c r="J26" s="213"/>
-      <c r="K26" s="182"/>
+      <c r="J26" s="210"/>
+      <c r="K26" s="176"/>
       <c r="L26" s="8" t="s">
         <v>112</v>
       </c>
@@ -64716,12 +64719,12 @@
       <c r="E28" s="98"/>
       <c r="F28" s="102">
         <f>AVERAGE(F6:F26)</f>
-        <v>32.852231578947368</v>
+        <v>14.506738947368424</v>
       </c>
       <c r="G28" s="97"/>
       <c r="H28" s="102">
         <f>AVERAGE(H6:H26)</f>
-        <v>35.902209473684216</v>
+        <v>17.556716842105264</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -64734,12 +64737,12 @@
       <c r="E29" s="98"/>
       <c r="F29" s="102">
         <f>STDEV(F6:F26)</f>
-        <v>84.305099412433663</v>
+        <v>34.672079293559328</v>
       </c>
       <c r="G29" s="97"/>
       <c r="H29" s="102">
         <f>STDEV(H6:H26)</f>
-        <v>82.981927477811922</v>
+        <v>33.150072640569825</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -64754,7 +64757,7 @@
       <c r="G30" s="97"/>
       <c r="H30" s="102">
         <f>MEDIAN(H6:H26)</f>
-        <v>7.9423300000000001</v>
+        <v>3.9573299999999998</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -64769,7 +64772,7 @@
       <c r="G31" s="97"/>
       <c r="H31" s="97">
         <f>PERCENTRANK(H6:H26,16)</f>
-        <v>0.78300000000000003</v>
+        <v>0.83899999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -64778,7 +64781,7 @@
       </c>
       <c r="H32" s="47">
         <f>PERCENTILE(H6:H26,0.9)</f>
-        <v>100.36643599999998</v>
+        <v>34.921197999999947</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -64787,11 +64790,22 @@
       </c>
       <c r="H33" s="47">
         <f>PERCENTILE(H6:H20,0.9)</f>
-        <v>14.040621999999999</v>
+        <v>11.614180000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A6:A20"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="K25:K26"/>
@@ -64799,17 +64813,6 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="J6:J20"/>
     <mergeCell ref="J21:J26"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A6:A20"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -64823,8 +64826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -64841,26 +64844,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="K1" s="215" t="s">
+      <c r="K1" s="221" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="215"/>
+      <c r="L1" s="221"/>
       <c r="N1" s="87" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="12" customFormat="1" ht="25.5" customHeight="1">
       <c r="C2" s="4"/>
-      <c r="D2" s="214" t="s">
+      <c r="D2" s="220" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="214"/>
-      <c r="F2" s="214"/>
-      <c r="G2" s="214" t="s">
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="214"/>
-      <c r="I2" s="214"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
       <c r="K2" s="84" t="s">
         <v>137</v>
       </c>
@@ -64871,13 +64874,13 @@
       <c r="N2" s="90"/>
     </row>
     <row r="3" spans="1:15" s="12" customFormat="1" ht="25.5">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="171" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="202" t="s">
+      <c r="B3" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="182" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="33" t="s">
@@ -64908,9 +64911,9 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="13" customFormat="1" ht="25.5">
-      <c r="A4" s="172"/>
-      <c r="B4" s="172"/>
-      <c r="C4" s="172"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
       <c r="D4" s="35" t="s">
         <v>49</v>
       </c>
@@ -64939,7 +64942,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="200" t="s">
+      <c r="A5" s="172" t="s">
         <v>157</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -64988,7 +64991,7 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="201"/>
+      <c r="A6" s="173"/>
       <c r="B6" s="8" t="s">
         <v>29</v>
       </c>
@@ -65027,7 +65030,7 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="201"/>
+      <c r="A7" s="173"/>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
@@ -65066,7 +65069,7 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="201"/>
+      <c r="A8" s="173"/>
       <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
@@ -65105,7 +65108,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="201"/>
+      <c r="A9" s="173"/>
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
@@ -65144,7 +65147,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="201"/>
+      <c r="A10" s="173"/>
       <c r="B10" s="8" t="s">
         <v>32</v>
       </c>
@@ -65183,7 +65186,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="201"/>
+      <c r="A11" s="173"/>
       <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
@@ -65222,7 +65225,7 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="201"/>
+      <c r="A12" s="173"/>
       <c r="B12" s="8" t="s">
         <v>36</v>
       </c>
@@ -65261,7 +65264,7 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="201"/>
+      <c r="A13" s="173"/>
       <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
@@ -65300,7 +65303,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="201"/>
+      <c r="A14" s="173"/>
       <c r="B14" s="8" t="s">
         <v>26</v>
       </c>
@@ -65339,7 +65342,7 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="201"/>
+      <c r="A15" s="173"/>
       <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
@@ -65378,7 +65381,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="201"/>
+      <c r="A16" s="173"/>
       <c r="B16" s="8" t="s">
         <v>28</v>
       </c>
@@ -65417,7 +65420,7 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="201"/>
+      <c r="A17" s="173"/>
       <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
@@ -65456,7 +65459,7 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="201"/>
+      <c r="A18" s="173"/>
       <c r="B18" s="8" t="s">
         <v>35</v>
       </c>
@@ -65495,7 +65498,7 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="201"/>
+      <c r="A19" s="173"/>
       <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
@@ -65583,10 +65586,10 @@
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="173" t="s">
+      <c r="A21" s="185" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="187" t="s">
+      <c r="B21" s="171" t="s">
         <v>129</v>
       </c>
       <c r="C21" s="53" t="s">
@@ -65634,8 +65637,8 @@
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="184"/>
-      <c r="B22" s="188"/>
+      <c r="A22" s="193"/>
+      <c r="B22" s="170"/>
       <c r="C22" s="53" t="s">
         <v>117</v>
       </c>
@@ -65673,8 +65676,8 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="184"/>
-      <c r="B23" s="188"/>
+      <c r="A23" s="193"/>
+      <c r="B23" s="170"/>
       <c r="C23" s="55" t="s">
         <v>121</v>
       </c>
@@ -65703,8 +65706,8 @@
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="184"/>
-      <c r="B24" s="188"/>
+      <c r="A24" s="193"/>
+      <c r="B24" s="170"/>
       <c r="C24" s="53" t="s">
         <v>120</v>
       </c>
@@ -65733,8 +65736,8 @@
       </c>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="174"/>
-      <c r="B25" s="187" t="s">
+      <c r="A25" s="186"/>
+      <c r="B25" s="171" t="s">
         <v>130</v>
       </c>
       <c r="C25" s="53" t="s">
@@ -65774,8 +65777,8 @@
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="174"/>
-      <c r="B26" s="188"/>
+      <c r="A26" s="186"/>
+      <c r="B26" s="170"/>
       <c r="C26" s="53" t="s">
         <v>117</v>
       </c>
@@ -65813,8 +65816,8 @@
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="174"/>
-      <c r="B27" s="188"/>
+      <c r="A27" s="186"/>
+      <c r="B27" s="170"/>
       <c r="C27" s="53" t="s">
         <v>117</v>
       </c>
@@ -65843,8 +65846,8 @@
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="174"/>
-      <c r="B28" s="188"/>
+      <c r="A28" s="186"/>
+      <c r="B28" s="170"/>
       <c r="C28" s="55" t="s">
         <v>121</v>
       </c>
@@ -65873,8 +65876,8 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="175"/>
-      <c r="B29" s="188"/>
+      <c r="A29" s="187"/>
+      <c r="B29" s="170"/>
       <c r="C29" s="53" t="s">
         <v>120</v>
       </c>
@@ -65903,13 +65906,13 @@
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="173" t="s">
+      <c r="A30" s="185" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="220" t="s">
+      <c r="B30" s="218" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="218" t="s">
+      <c r="C30" s="216" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="14">
@@ -65939,15 +65942,12 @@
         <f>AVERAGE(K30:K33)</f>
         <v>21.948207500000002</v>
       </c>
-      <c r="O30" s="47" t="e">
-        <f>AVERAGE(L30:L33)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="O30" s="47"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="174"/>
-      <c r="B31" s="221"/>
-      <c r="C31" s="219"/>
+      <c r="A31" s="186"/>
+      <c r="B31" s="219"/>
+      <c r="C31" s="217"/>
       <c r="D31" s="14">
         <f>'Sorted Output'!H469</f>
         <v>-0.1963</v>
@@ -65973,11 +65973,11 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="174"/>
-      <c r="B32" s="220" t="s">
+      <c r="A32" s="186"/>
+      <c r="B32" s="218" t="s">
         <v>126</v>
       </c>
-      <c r="C32" s="218" t="s">
+      <c r="C32" s="216" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="14">
@@ -66005,9 +66005,9 @@
       </c>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="175"/>
-      <c r="B33" s="221"/>
-      <c r="C33" s="219"/>
+      <c r="A33" s="187"/>
+      <c r="B33" s="219"/>
+      <c r="C33" s="217"/>
       <c r="D33" s="14">
         <f>'Sorted Output'!H471</f>
         <v>-0.10009999999999999</v>
@@ -66033,10 +66033,10 @@
       </c>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="216" t="s">
+      <c r="A34" s="214" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="217"/>
+      <c r="B34" s="215"/>
       <c r="C34" s="9"/>
       <c r="D34" s="14">
         <f>'Sorted Output'!H496</f>
@@ -66197,6 +66197,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C32:C33"/>
@@ -66207,12 +66213,6 @@
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B25:B29"/>
     <mergeCell ref="A21:A29"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>